<commit_message>
DDT(get Data from Excel)-HR
</commit_message>
<xml_diff>
--- a/Payload/test_Data/TestData.xlsx
+++ b/Payload/test_Data/TestData.xlsx
@@ -5,15 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arshad Mehmood\OneDrive - Riphah International University\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arshad Mehmood\OneDrive - Riphah International University\Desktop\MPOPlayWright\Payload\test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF2948F-0C63-419F-A779-85A6F7AD6977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28220DF9-C5C3-4D74-A82D-5F8565B5ED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CompanyHoliday" sheetId="1" r:id="rId1"/>
+    <sheet name="CommentTemplates" sheetId="2" r:id="rId2"/>
+    <sheet name="CriteriaLibrary" sheetId="3" r:id="rId3"/>
+    <sheet name="EmployeeSuccession" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +28,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Holiday Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>National Holiday</t>
+  </si>
+  <si>
+    <t>1/22/2025</t>
+  </si>
+  <si>
+    <t>Holiday Name2</t>
+  </si>
+  <si>
+    <t>Date1</t>
+  </si>
+  <si>
+    <t>Holiday Name1</t>
+  </si>
+  <si>
+    <t>Date2</t>
+  </si>
+  <si>
+    <t>New Year</t>
+  </si>
+  <si>
+    <t>1/1/2025</t>
+  </si>
+  <si>
+    <t>Comment Name</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Test Comments(Added by Automation)</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Succession</t>
+  </si>
+  <si>
+    <t>Rediness</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>amy</t>
+  </si>
+  <si>
+    <t>re</t>
+  </si>
+  <si>
+    <t>Testing add note succession(Added by Automation)</t>
   </si>
 </sst>
 </file>
@@ -72,9 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,26 +414,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B100B664-FFAE-4560-A173-D34EFD0BC0FB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2CE3E0-B99C-4F95-95E3-9AEDE254C032}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A95774-DF39-4551-80F7-17254C4273C0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>